<commit_message>
added cashflow, separate by year and together
</commit_message>
<xml_diff>
--- a/input/Financial Statement WMT/Compiled Income Statement-WMT.xlsx
+++ b/input/Financial Statement WMT/Compiled Income Statement-WMT.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,122 +441,107 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Q3 2018</t>
+          <t>Year Ended 2018</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Q4 2018</t>
+          <t>Q1 2019</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Year Ended 2018</t>
+          <t>Q2 2019</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Q1 2019</t>
+          <t>Q3 2019</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Q2 2019</t>
+          <t>Q4 2019</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Q3 2019</t>
+          <t>Year Ended 2019</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Q4 2019</t>
+          <t>Q1 2020</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Year Ended 2019</t>
+          <t>Q2 2020</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Q1 2020</t>
+          <t>Q3 2020</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Q2 2020</t>
+          <t>Q4 2020</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Q3 2020</t>
+          <t>Year Ended 2020</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Q4 2020</t>
+          <t>Q1 2021</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Year Ended 2020</t>
+          <t>Q2 2021</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Q1 2021</t>
+          <t>Q3 2021</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Q2 2021</t>
+          <t>Q4 2021</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Q3 2021</t>
+          <t>Year Ended 2021</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Q4 2021</t>
+          <t>Q1 2022</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Year Ended 2021</t>
+          <t>Q2 2022</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Q1 2022</t>
+          <t>Q3 2022</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Q2 2022</t>
+          <t>Q4 2022</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Q3 2022</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Q4 2022</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
           <t>Year Ended 2022</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Q1 2023</t>
         </is>
       </c>
     </row>
@@ -587,9 +572,6 @@
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,76 +580,67 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>122136</v>
+        <v>495761</v>
       </c>
       <c r="C3" t="n">
-        <v>373625</v>
+        <v>121630</v>
       </c>
       <c r="D3" t="n">
-        <v>495761</v>
+        <v>127059</v>
       </c>
       <c r="E3" t="n">
-        <v>121630</v>
+        <v>123897</v>
       </c>
       <c r="F3" t="n">
-        <v>127059</v>
+        <v>386432</v>
       </c>
       <c r="G3" t="n">
-        <v>123897</v>
+        <v>510329</v>
       </c>
       <c r="H3" t="n">
-        <v>386432</v>
+        <v>122949</v>
       </c>
       <c r="I3" t="n">
-        <v>510329</v>
+        <v>129388</v>
       </c>
       <c r="J3" t="n">
-        <v>122949</v>
+        <v>126981</v>
       </c>
       <c r="K3" t="n">
-        <v>129388</v>
+        <v>392945</v>
       </c>
       <c r="L3" t="n">
-        <v>126981</v>
+        <v>519926</v>
       </c>
       <c r="M3" t="n">
-        <v>392945</v>
+        <v>133672</v>
       </c>
       <c r="N3" t="n">
-        <v>519926</v>
+        <v>136824</v>
       </c>
       <c r="O3" t="n">
-        <v>133672</v>
+        <v>133752</v>
       </c>
       <c r="P3" t="n">
-        <v>136824</v>
+        <v>421481</v>
       </c>
       <c r="Q3" t="n">
-        <v>133752</v>
+        <v>555233</v>
       </c>
       <c r="R3" t="n">
-        <v>421481</v>
+        <v>137159</v>
       </c>
       <c r="S3" t="n">
-        <v>555233</v>
+        <v>139871</v>
       </c>
       <c r="T3" t="n">
-        <v>137159</v>
+        <v>139207</v>
       </c>
       <c r="U3" t="n">
-        <v>139871</v>
+        <v>428555</v>
       </c>
       <c r="V3" t="n">
-        <v>139207</v>
-      </c>
-      <c r="W3" t="n">
-        <v>428555</v>
-      </c>
-      <c r="X3" t="n">
         <v>567762</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>140288</v>
       </c>
     </row>
     <row r="4">
@@ -677,76 +650,67 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1043</v>
+        <v>4582</v>
       </c>
       <c r="C4" t="n">
-        <v>3539</v>
+        <v>1060</v>
       </c>
       <c r="D4" t="n">
-        <v>4582</v>
+        <v>969</v>
       </c>
       <c r="E4" t="n">
-        <v>1060</v>
+        <v>997</v>
       </c>
       <c r="F4" t="n">
-        <v>969</v>
+        <v>3079</v>
       </c>
       <c r="G4" t="n">
-        <v>997</v>
+        <v>4076</v>
       </c>
       <c r="H4" t="n">
-        <v>3079</v>
+        <v>976</v>
       </c>
       <c r="I4" t="n">
-        <v>4076</v>
+        <v>989</v>
       </c>
       <c r="J4" t="n">
-        <v>976</v>
+        <v>1010</v>
       </c>
       <c r="K4" t="n">
-        <v>989</v>
+        <v>3028</v>
       </c>
       <c r="L4" t="n">
-        <v>1010</v>
+        <v>4038</v>
       </c>
       <c r="M4" t="n">
-        <v>3028</v>
+        <v>950</v>
       </c>
       <c r="N4" t="n">
-        <v>4038</v>
+        <v>918</v>
       </c>
       <c r="O4" t="n">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="P4" t="n">
-        <v>918</v>
+        <v>2962</v>
       </c>
       <c r="Q4" t="n">
-        <v>956</v>
+        <v>3918</v>
       </c>
       <c r="R4" t="n">
-        <v>2962</v>
+        <v>1151</v>
       </c>
       <c r="S4" t="n">
-        <v>3918</v>
+        <v>1177</v>
       </c>
       <c r="T4" t="n">
-        <v>1151</v>
+        <v>1318</v>
       </c>
       <c r="U4" t="n">
-        <v>1177</v>
+        <v>3674</v>
       </c>
       <c r="V4" t="n">
-        <v>1318</v>
-      </c>
-      <c r="W4" t="n">
-        <v>3674</v>
-      </c>
-      <c r="X4" t="n">
         <v>4992</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>1281</v>
       </c>
     </row>
     <row r="5">
@@ -756,76 +720,67 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>123179</v>
+        <v>500343</v>
       </c>
       <c r="C5" t="n">
-        <v>377164</v>
+        <v>122690</v>
       </c>
       <c r="D5" t="n">
-        <v>500343</v>
+        <v>128028</v>
       </c>
       <c r="E5" t="n">
-        <v>122690</v>
+        <v>124894</v>
       </c>
       <c r="F5" t="n">
-        <v>128028</v>
+        <v>389511</v>
       </c>
       <c r="G5" t="n">
-        <v>124894</v>
+        <v>514405</v>
       </c>
       <c r="H5" t="n">
-        <v>389511</v>
+        <v>123925</v>
       </c>
       <c r="I5" t="n">
-        <v>514405</v>
+        <v>130377</v>
       </c>
       <c r="J5" t="n">
-        <v>123925</v>
+        <v>127991</v>
       </c>
       <c r="K5" t="n">
-        <v>130377</v>
+        <v>395973</v>
       </c>
       <c r="L5" t="n">
-        <v>127991</v>
+        <v>523964</v>
       </c>
       <c r="M5" t="n">
-        <v>395973</v>
+        <v>134622</v>
       </c>
       <c r="N5" t="n">
-        <v>523964</v>
+        <v>137742</v>
       </c>
       <c r="O5" t="n">
-        <v>134622</v>
+        <v>134708</v>
       </c>
       <c r="P5" t="n">
-        <v>137742</v>
+        <v>424443</v>
       </c>
       <c r="Q5" t="n">
-        <v>134708</v>
+        <v>559151</v>
       </c>
       <c r="R5" t="n">
-        <v>424443</v>
+        <v>138310</v>
       </c>
       <c r="S5" t="n">
-        <v>559151</v>
+        <v>141048</v>
       </c>
       <c r="T5" t="n">
-        <v>138310</v>
+        <v>140525</v>
       </c>
       <c r="U5" t="n">
-        <v>141048</v>
+        <v>432229</v>
       </c>
       <c r="V5" t="n">
-        <v>140525</v>
-      </c>
-      <c r="W5" t="n">
-        <v>432229</v>
-      </c>
-      <c r="X5" t="n">
         <v>572754</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>141569</v>
       </c>
     </row>
     <row r="6">
@@ -855,9 +810,6 @@
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -866,76 +818,67 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>91547</v>
+        <v>373396</v>
       </c>
       <c r="C7" t="n">
-        <v>281849</v>
+        <v>91707</v>
       </c>
       <c r="D7" t="n">
-        <v>373396</v>
+        <v>95571</v>
       </c>
       <c r="E7" t="n">
-        <v>91707</v>
+        <v>93116</v>
       </c>
       <c r="F7" t="n">
-        <v>95571</v>
+        <v>292185</v>
       </c>
       <c r="G7" t="n">
-        <v>93116</v>
+        <v>385301</v>
       </c>
       <c r="H7" t="n">
-        <v>292185</v>
+        <v>93034</v>
       </c>
       <c r="I7" t="n">
-        <v>385301</v>
+        <v>97923</v>
       </c>
       <c r="J7" t="n">
-        <v>93034</v>
+        <v>95900</v>
       </c>
       <c r="K7" t="n">
-        <v>97923</v>
+        <v>298705</v>
       </c>
       <c r="L7" t="n">
-        <v>95900</v>
+        <v>394605</v>
       </c>
       <c r="M7" t="n">
-        <v>298705</v>
+        <v>102026</v>
       </c>
       <c r="N7" t="n">
-        <v>394605</v>
+        <v>102689</v>
       </c>
       <c r="O7" t="n">
-        <v>102026</v>
+        <v>100339</v>
       </c>
       <c r="P7" t="n">
-        <v>102689</v>
+        <v>319976</v>
       </c>
       <c r="Q7" t="n">
-        <v>100339</v>
+        <v>420315</v>
       </c>
       <c r="R7" t="n">
-        <v>319976</v>
+        <v>103272</v>
       </c>
       <c r="S7" t="n">
-        <v>420315</v>
+        <v>105183</v>
       </c>
       <c r="T7" t="n">
-        <v>103272</v>
+        <v>105023</v>
       </c>
       <c r="U7" t="n">
-        <v>105183</v>
+        <v>323977</v>
       </c>
       <c r="V7" t="n">
-        <v>105023</v>
-      </c>
-      <c r="W7" t="n">
-        <v>323977</v>
-      </c>
-      <c r="X7" t="n">
         <v>429000</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>106847</v>
       </c>
     </row>
     <row r="8">
@@ -945,76 +888,67 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>26868</v>
+        <v>106510</v>
       </c>
       <c r="C8" t="n">
-        <v>79642</v>
+        <v>25829</v>
       </c>
       <c r="D8" t="n">
-        <v>106510</v>
+        <v>26707</v>
       </c>
       <c r="E8" t="n">
-        <v>25829</v>
+        <v>26792</v>
       </c>
       <c r="F8" t="n">
-        <v>26707</v>
+        <v>80355</v>
       </c>
       <c r="G8" t="n">
-        <v>26792</v>
+        <v>107147</v>
       </c>
       <c r="H8" t="n">
-        <v>80355</v>
+        <v>25946</v>
       </c>
       <c r="I8" t="n">
-        <v>107147</v>
+        <v>26871</v>
       </c>
       <c r="J8" t="n">
-        <v>25946</v>
+        <v>27373</v>
       </c>
       <c r="K8" t="n">
-        <v>26871</v>
+        <v>81418</v>
       </c>
       <c r="L8" t="n">
-        <v>27373</v>
+        <v>108791</v>
       </c>
       <c r="M8" t="n">
-        <v>81418</v>
+        <v>27372</v>
       </c>
       <c r="N8" t="n">
-        <v>108791</v>
+        <v>28994</v>
       </c>
       <c r="O8" t="n">
-        <v>27372</v>
+        <v>28591</v>
       </c>
       <c r="P8" t="n">
-        <v>28994</v>
+        <v>87697</v>
       </c>
       <c r="Q8" t="n">
-        <v>28591</v>
+        <v>116288</v>
       </c>
       <c r="R8" t="n">
-        <v>87697</v>
+        <v>28129</v>
       </c>
       <c r="S8" t="n">
-        <v>116288</v>
+        <v>28511</v>
       </c>
       <c r="T8" t="n">
-        <v>28129</v>
+        <v>29710</v>
       </c>
       <c r="U8" t="n">
-        <v>28511</v>
+        <v>88102</v>
       </c>
       <c r="V8" t="n">
-        <v>29710</v>
-      </c>
-      <c r="W8" t="n">
-        <v>88102</v>
-      </c>
-      <c r="X8" t="n">
         <v>117812</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>29404</v>
       </c>
     </row>
     <row r="9">
@@ -1024,76 +958,67 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4764</v>
+        <v>20437</v>
       </c>
       <c r="C9" t="n">
-        <v>15673</v>
+        <v>5154</v>
       </c>
       <c r="D9" t="n">
-        <v>20437</v>
+        <v>5750</v>
       </c>
       <c r="E9" t="n">
-        <v>5154</v>
+        <v>4986</v>
       </c>
       <c r="F9" t="n">
-        <v>5750</v>
+        <v>16971</v>
       </c>
       <c r="G9" t="n">
-        <v>4986</v>
+        <v>21957</v>
       </c>
       <c r="H9" t="n">
-        <v>16971</v>
+        <v>4945</v>
       </c>
       <c r="I9" t="n">
-        <v>21957</v>
+        <v>5583</v>
       </c>
       <c r="J9" t="n">
-        <v>4945</v>
+        <v>4718</v>
       </c>
       <c r="K9" t="n">
-        <v>5583</v>
+        <v>15850</v>
       </c>
       <c r="L9" t="n">
-        <v>4718</v>
+        <v>20568</v>
       </c>
       <c r="M9" t="n">
-        <v>15850</v>
+        <v>5224</v>
       </c>
       <c r="N9" t="n">
-        <v>20568</v>
+        <v>6059</v>
       </c>
       <c r="O9" t="n">
-        <v>5224</v>
+        <v>5778</v>
       </c>
       <c r="P9" t="n">
-        <v>6059</v>
+        <v>16770</v>
       </c>
       <c r="Q9" t="n">
-        <v>5778</v>
+        <v>22548</v>
       </c>
       <c r="R9" t="n">
-        <v>16770</v>
+        <v>6909</v>
       </c>
       <c r="S9" t="n">
-        <v>22548</v>
+        <v>7354</v>
       </c>
       <c r="T9" t="n">
-        <v>6909</v>
+        <v>5792</v>
       </c>
       <c r="U9" t="n">
-        <v>7354</v>
+        <v>20150</v>
       </c>
       <c r="V9" t="n">
-        <v>5792</v>
-      </c>
-      <c r="W9" t="n">
-        <v>20150</v>
-      </c>
-      <c r="X9" t="n">
         <v>25942</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>5318</v>
       </c>
     </row>
     <row r="10">
@@ -1123,9 +1048,6 @@
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1134,76 +1056,67 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>502</v>
+        <v>1978</v>
       </c>
       <c r="C11" t="n">
-        <v>1476</v>
+        <v>437</v>
       </c>
       <c r="D11" t="n">
-        <v>1978</v>
+        <v>460</v>
       </c>
       <c r="E11" t="n">
+        <v>501</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1474</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1975</v>
+      </c>
+      <c r="H11" t="n">
+        <v>588</v>
+      </c>
+      <c r="I11" t="n">
+        <v>558</v>
+      </c>
+      <c r="J11" t="n">
+        <v>547</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1715</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2262</v>
+      </c>
+      <c r="M11" t="n">
+        <v>510</v>
+      </c>
+      <c r="N11" t="n">
+        <v>577</v>
+      </c>
+      <c r="O11" t="n">
+        <v>455</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1521</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1976</v>
+      </c>
+      <c r="R11" t="n">
+        <v>481</v>
+      </c>
+      <c r="S11" t="n">
         <v>437</v>
       </c>
-      <c r="F11" t="n">
-        <v>460</v>
-      </c>
-      <c r="G11" t="n">
-        <v>501</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1474</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1975</v>
-      </c>
-      <c r="J11" t="n">
-        <v>588</v>
-      </c>
-      <c r="K11" t="n">
-        <v>558</v>
-      </c>
-      <c r="L11" t="n">
-        <v>547</v>
-      </c>
-      <c r="M11" t="n">
-        <v>1715</v>
-      </c>
-      <c r="N11" t="n">
-        <v>2262</v>
-      </c>
-      <c r="O11" t="n">
-        <v>510</v>
-      </c>
-      <c r="P11" t="n">
-        <v>577</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>455</v>
-      </c>
-      <c r="R11" t="n">
-        <v>1521</v>
-      </c>
-      <c r="S11" t="n">
-        <v>1976</v>
-      </c>
       <c r="T11" t="n">
-        <v>481</v>
+        <v>408</v>
       </c>
       <c r="U11" t="n">
-        <v>437</v>
+        <v>1266</v>
       </c>
       <c r="V11" t="n">
-        <v>408</v>
-      </c>
-      <c r="W11" t="n">
-        <v>1266</v>
-      </c>
-      <c r="X11" t="n">
         <v>1674</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>372</v>
       </c>
     </row>
     <row r="12">
@@ -1213,29 +1126,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>81</v>
+        <v>352</v>
       </c>
       <c r="C12" t="n">
-        <v>271</v>
+        <v>93</v>
       </c>
       <c r="D12" t="n">
-        <v>352</v>
+        <v>94</v>
       </c>
       <c r="E12" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" t="n">
-        <v>94</v>
+        <v>279</v>
       </c>
       <c r="G12" t="n">
-        <v>92</v>
-      </c>
-      <c r="H12" t="n">
-        <v>279</v>
-      </c>
-      <c r="I12" t="n">
         <v>371</v>
       </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1249,9 +1158,6 @@
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1265,36 +1171,33 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>85</v>
+      </c>
+      <c r="I13" t="n">
+        <v>83</v>
+      </c>
       <c r="J13" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K13" t="n">
-        <v>83</v>
+        <v>251</v>
       </c>
       <c r="L13" t="n">
-        <v>86</v>
-      </c>
-      <c r="M13" t="n">
-        <v>251</v>
-      </c>
-      <c r="N13" t="n">
         <v>337</v>
       </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+      <c r="Q13" t="n">
+        <v>339</v>
+      </c>
       <c r="R13" t="inlineStr"/>
-      <c r="S13" t="n">
-        <v>339</v>
-      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1313,36 +1216,31 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>82</v>
+      </c>
+      <c r="N14" t="n">
+        <v>81</v>
+      </c>
       <c r="O14" t="n">
-        <v>82</v>
-      </c>
-      <c r="P14" t="n">
-        <v>81</v>
-      </c>
-      <c r="Q14" t="n">
         <v>86</v>
       </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="n">
+        <v>85</v>
+      </c>
+      <c r="S14" t="n">
+        <v>78</v>
+      </c>
       <c r="T14" t="n">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="U14" t="n">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="V14" t="n">
-        <v>78</v>
-      </c>
-      <c r="W14" t="n">
-        <v>242</v>
-      </c>
-      <c r="X14" t="n">
         <v>320</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>83</v>
       </c>
     </row>
     <row r="15">
@@ -1352,76 +1250,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-42</v>
+        <v>-152</v>
       </c>
       <c r="C15" t="n">
-        <v>-110</v>
+        <v>-43</v>
       </c>
       <c r="D15" t="n">
-        <v>-152</v>
+        <v>-51</v>
       </c>
       <c r="E15" t="n">
+        <v>-59</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-158</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-217</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-48</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-56</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-44</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-145</v>
+      </c>
+      <c r="L15" t="n">
+        <v>-189</v>
+      </c>
+      <c r="M15" t="n">
         <v>-43</v>
       </c>
-      <c r="F15" t="n">
-        <v>-51</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-59</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="N15" t="n">
+        <v>-23</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-25</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-96</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-121</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-30</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-37</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-44</v>
+      </c>
+      <c r="U15" t="n">
+        <v>-114</v>
+      </c>
+      <c r="V15" t="n">
         <v>-158</v>
-      </c>
-      <c r="I15" t="n">
-        <v>-217</v>
-      </c>
-      <c r="J15" t="n">
-        <v>-48</v>
-      </c>
-      <c r="K15" t="n">
-        <v>-56</v>
-      </c>
-      <c r="L15" t="n">
-        <v>-44</v>
-      </c>
-      <c r="M15" t="n">
-        <v>-145</v>
-      </c>
-      <c r="N15" t="n">
-        <v>-189</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-43</v>
-      </c>
-      <c r="P15" t="n">
-        <v>-23</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>-25</v>
-      </c>
-      <c r="R15" t="n">
-        <v>-96</v>
-      </c>
-      <c r="S15" t="n">
-        <v>-121</v>
-      </c>
-      <c r="T15" t="n">
-        <v>-30</v>
-      </c>
-      <c r="U15" t="n">
-        <v>-37</v>
-      </c>
-      <c r="V15" t="n">
-        <v>-44</v>
-      </c>
-      <c r="W15" t="n">
-        <v>-114</v>
-      </c>
-      <c r="X15" t="n">
-        <v>-158</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>-36</v>
       </c>
     </row>
     <row r="16">
@@ -1431,76 +1320,67 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>541</v>
+        <v>2178</v>
       </c>
       <c r="C16" t="n">
-        <v>1637</v>
+        <v>487</v>
       </c>
       <c r="D16" t="n">
-        <v>2178</v>
+        <v>503</v>
       </c>
       <c r="E16" t="n">
-        <v>487</v>
+        <v>534</v>
       </c>
       <c r="F16" t="n">
-        <v>503</v>
+        <v>1595</v>
       </c>
       <c r="G16" t="n">
-        <v>534</v>
+        <v>2129</v>
       </c>
       <c r="H16" t="n">
-        <v>1595</v>
+        <v>625</v>
       </c>
       <c r="I16" t="n">
-        <v>2129</v>
+        <v>585</v>
       </c>
       <c r="J16" t="n">
-        <v>625</v>
+        <v>589</v>
       </c>
       <c r="K16" t="n">
-        <v>585</v>
+        <v>1821</v>
       </c>
       <c r="L16" t="n">
-        <v>589</v>
+        <v>2410</v>
       </c>
       <c r="M16" t="n">
-        <v>1821</v>
+        <v>549</v>
       </c>
       <c r="N16" t="n">
-        <v>2410</v>
+        <v>635</v>
       </c>
       <c r="O16" t="n">
-        <v>549</v>
+        <v>516</v>
       </c>
       <c r="P16" t="n">
-        <v>635</v>
+        <v>1678</v>
       </c>
       <c r="Q16" t="n">
-        <v>516</v>
+        <v>2194</v>
       </c>
       <c r="R16" t="n">
-        <v>1678</v>
+        <v>536</v>
       </c>
       <c r="S16" t="n">
-        <v>2194</v>
+        <v>478</v>
       </c>
       <c r="T16" t="n">
-        <v>536</v>
+        <v>442</v>
       </c>
       <c r="U16" t="n">
-        <v>478</v>
+        <v>1394</v>
       </c>
       <c r="V16" t="n">
-        <v>442</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1394</v>
-      </c>
-      <c r="X16" t="n">
         <v>1836</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>419</v>
       </c>
     </row>
     <row r="17">
@@ -1510,51 +1390,44 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1344</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1792</v>
-      </c>
+        <v>3136</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>3136</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>2410</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
       <c r="V17" t="n">
         <v>2410</v>
       </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" t="n">
-        <v>2410</v>
-      </c>
-      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1563,11 +1436,11 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>1845</v>
+      </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>1845</v>
-      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
@@ -1585,9 +1458,6 @@
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1597,11 +1467,11 @@
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>-4849</v>
+      </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>-4849</v>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
@@ -1618,9 +1488,6 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1631,64 +1498,59 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>-1876</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10244</v>
+      </c>
       <c r="G20" t="n">
-        <v>-1876</v>
+        <v>8368</v>
       </c>
       <c r="H20" t="n">
-        <v>10244</v>
+        <v>-837</v>
       </c>
       <c r="I20" t="n">
-        <v>8368</v>
+        <v>85</v>
       </c>
       <c r="J20" t="n">
-        <v>-837</v>
+        <v>-244</v>
       </c>
       <c r="K20" t="n">
-        <v>85</v>
+        <v>-1714</v>
       </c>
       <c r="L20" t="n">
-        <v>-244</v>
+        <v>-1958</v>
       </c>
       <c r="M20" t="n">
-        <v>-1714</v>
+        <v>-721</v>
       </c>
       <c r="N20" t="n">
-        <v>-1958</v>
+        <v>-3222</v>
       </c>
       <c r="O20" t="n">
-        <v>-721</v>
+        <v>-1853</v>
       </c>
       <c r="P20" t="n">
-        <v>-3222</v>
+        <v>1643</v>
       </c>
       <c r="Q20" t="n">
-        <v>-1853</v>
+        <v>-210</v>
       </c>
       <c r="R20" t="n">
-        <v>1643</v>
+        <v>2529</v>
       </c>
       <c r="S20" t="n">
-        <v>-210</v>
+        <v>953</v>
       </c>
       <c r="T20" t="n">
-        <v>2529</v>
+        <v>-1207</v>
       </c>
       <c r="U20" t="n">
-        <v>953</v>
+        <v>4207</v>
       </c>
       <c r="V20" t="n">
-        <v>-1207</v>
-      </c>
-      <c r="W20" t="n">
-        <v>4207</v>
-      </c>
-      <c r="X20" t="n">
         <v>3000</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>1998</v>
       </c>
     </row>
     <row r="21">
@@ -1698,76 +1560,67 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2879</v>
+        <v>15123</v>
       </c>
       <c r="C21" t="n">
-        <v>12244</v>
+        <v>2822</v>
       </c>
       <c r="D21" t="n">
-        <v>15123</v>
+        <v>398</v>
       </c>
       <c r="E21" t="n">
-        <v>2822</v>
+        <v>2576</v>
       </c>
       <c r="F21" t="n">
-        <v>398</v>
+        <v>8884</v>
       </c>
       <c r="G21" t="n">
-        <v>2576</v>
+        <v>11460</v>
       </c>
       <c r="H21" t="n">
-        <v>8884</v>
+        <v>5157</v>
       </c>
       <c r="I21" t="n">
-        <v>11460</v>
+        <v>4913</v>
       </c>
       <c r="J21" t="n">
-        <v>5157</v>
+        <v>4373</v>
       </c>
       <c r="K21" t="n">
-        <v>4913</v>
+        <v>15743</v>
       </c>
       <c r="L21" t="n">
-        <v>4373</v>
+        <v>20116</v>
       </c>
       <c r="M21" t="n">
-        <v>15743</v>
+        <v>5396</v>
       </c>
       <c r="N21" t="n">
-        <v>20116</v>
+        <v>8646</v>
       </c>
       <c r="O21" t="n">
-        <v>5396</v>
+        <v>7115</v>
       </c>
       <c r="P21" t="n">
-        <v>8646</v>
+        <v>13449</v>
       </c>
       <c r="Q21" t="n">
-        <v>7115</v>
+        <v>20564</v>
       </c>
       <c r="R21" t="n">
-        <v>13449</v>
+        <v>3844</v>
       </c>
       <c r="S21" t="n">
-        <v>20564</v>
+        <v>5923</v>
       </c>
       <c r="T21" t="n">
-        <v>3844</v>
+        <v>4147</v>
       </c>
       <c r="U21" t="n">
-        <v>5923</v>
+        <v>14549</v>
       </c>
       <c r="V21" t="n">
-        <v>4147</v>
-      </c>
-      <c r="W21" t="n">
-        <v>14549</v>
-      </c>
-      <c r="X21" t="n">
         <v>18696</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>2901</v>
       </c>
     </row>
     <row r="22">
@@ -1777,76 +1630,67 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>975</v>
+        <v>4600</v>
       </c>
       <c r="C22" t="n">
-        <v>3625</v>
+        <v>546</v>
       </c>
       <c r="D22" t="n">
-        <v>4600</v>
+        <v>1125</v>
       </c>
       <c r="E22" t="n">
-        <v>546</v>
+        <v>759</v>
       </c>
       <c r="F22" t="n">
-        <v>1125</v>
+        <v>3522</v>
       </c>
       <c r="G22" t="n">
-        <v>759</v>
+        <v>4281</v>
       </c>
       <c r="H22" t="n">
-        <v>3522</v>
+        <v>1251</v>
       </c>
       <c r="I22" t="n">
-        <v>4281</v>
+        <v>1233</v>
       </c>
       <c r="J22" t="n">
-        <v>1251</v>
+        <v>1052</v>
       </c>
       <c r="K22" t="n">
-        <v>1233</v>
+        <v>3863</v>
       </c>
       <c r="L22" t="n">
-        <v>1052</v>
+        <v>4915</v>
       </c>
       <c r="M22" t="n">
-        <v>3863</v>
+        <v>1322</v>
       </c>
       <c r="N22" t="n">
-        <v>4915</v>
+        <v>2207</v>
       </c>
       <c r="O22" t="n">
-        <v>1322</v>
+        <v>1914</v>
       </c>
       <c r="P22" t="n">
-        <v>2207</v>
+        <v>4944</v>
       </c>
       <c r="Q22" t="n">
-        <v>1914</v>
+        <v>6858</v>
       </c>
       <c r="R22" t="n">
-        <v>4944</v>
+        <v>1033</v>
       </c>
       <c r="S22" t="n">
-        <v>6858</v>
+        <v>1559</v>
       </c>
       <c r="T22" t="n">
-        <v>1033</v>
+        <v>1015</v>
       </c>
       <c r="U22" t="n">
-        <v>1559</v>
+        <v>3741</v>
       </c>
       <c r="V22" t="n">
-        <v>1015</v>
-      </c>
-      <c r="W22" t="n">
-        <v>3741</v>
-      </c>
-      <c r="X22" t="n">
         <v>4756</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>798</v>
       </c>
     </row>
     <row r="23">
@@ -1856,76 +1700,67 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1904</v>
+        <v>10523</v>
       </c>
       <c r="C23" t="n">
-        <v>8619</v>
+        <v>2276</v>
       </c>
       <c r="D23" t="n">
-        <v>10523</v>
+        <v>-727</v>
       </c>
       <c r="E23" t="n">
-        <v>2276</v>
+        <v>1817</v>
       </c>
       <c r="F23" t="n">
-        <v>-727</v>
+        <v>5362</v>
       </c>
       <c r="G23" t="n">
-        <v>1817</v>
+        <v>7179</v>
       </c>
       <c r="H23" t="n">
-        <v>5362</v>
+        <v>3906</v>
       </c>
       <c r="I23" t="n">
-        <v>7179</v>
+        <v>3680</v>
       </c>
       <c r="J23" t="n">
-        <v>3906</v>
+        <v>3321</v>
       </c>
       <c r="K23" t="n">
-        <v>3680</v>
+        <v>11880</v>
       </c>
       <c r="L23" t="n">
-        <v>3321</v>
+        <v>15201</v>
       </c>
       <c r="M23" t="n">
-        <v>11880</v>
+        <v>4074</v>
       </c>
       <c r="N23" t="n">
-        <v>15201</v>
+        <v>6439</v>
       </c>
       <c r="O23" t="n">
-        <v>4074</v>
+        <v>5201</v>
       </c>
       <c r="P23" t="n">
-        <v>6439</v>
+        <v>8505</v>
       </c>
       <c r="Q23" t="n">
-        <v>5201</v>
+        <v>13706</v>
       </c>
       <c r="R23" t="n">
-        <v>8505</v>
+        <v>2811</v>
       </c>
       <c r="S23" t="n">
-        <v>13706</v>
+        <v>4364</v>
       </c>
       <c r="T23" t="n">
-        <v>2811</v>
+        <v>3132</v>
       </c>
       <c r="U23" t="n">
-        <v>4364</v>
+        <v>10808</v>
       </c>
       <c r="V23" t="n">
-        <v>3132</v>
-      </c>
-      <c r="W23" t="n">
-        <v>10808</v>
-      </c>
-      <c r="X23" t="n">
         <v>13940</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>2103</v>
       </c>
     </row>
     <row r="24">
@@ -1935,72 +1770,63 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-155</v>
+        <v>-661</v>
       </c>
       <c r="C24" t="n">
-        <v>-506</v>
+        <v>-142</v>
       </c>
       <c r="D24" t="n">
-        <v>-661</v>
+        <v>-134</v>
       </c>
       <c r="E24" t="n">
-        <v>-142</v>
+        <v>-107</v>
       </c>
       <c r="F24" t="n">
-        <v>-134</v>
+        <v>-402</v>
       </c>
       <c r="G24" t="n">
-        <v>-107</v>
+        <v>-509</v>
       </c>
       <c r="H24" t="n">
-        <v>-402</v>
+        <v>-64</v>
       </c>
       <c r="I24" t="n">
-        <v>-509</v>
+        <v>-70</v>
       </c>
       <c r="J24" t="n">
-        <v>-64</v>
+        <v>-33</v>
       </c>
       <c r="K24" t="n">
-        <v>-70</v>
+        <v>-287</v>
       </c>
       <c r="L24" t="n">
-        <v>-33</v>
+        <v>-320</v>
       </c>
       <c r="M24" t="n">
-        <v>-287</v>
-      </c>
-      <c r="N24" t="n">
-        <v>-320</v>
-      </c>
+        <v>-84</v>
+      </c>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-84</v>
-      </c>
-      <c r="P24" t="inlineStr"/>
+        <v>-66</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-130</v>
+      </c>
       <c r="Q24" t="n">
-        <v>-66</v>
+        <v>-196</v>
       </c>
       <c r="R24" t="n">
-        <v>-130</v>
-      </c>
-      <c r="S24" t="n">
-        <v>-196</v>
-      </c>
+        <v>-81</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="n">
-        <v>-81</v>
-      </c>
-      <c r="U24" t="inlineStr"/>
+        <v>-27</v>
+      </c>
+      <c r="U24" t="n">
+        <v>-240</v>
+      </c>
       <c r="V24" t="n">
-        <v>-27</v>
-      </c>
-      <c r="W24" t="n">
-        <v>-240</v>
-      </c>
-      <c r="X24" t="n">
         <v>-267</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>-49</v>
       </c>
     </row>
     <row r="25">
@@ -2021,22 +1847,19 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>37</v>
+      </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
-        <v>37</v>
-      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="n">
+        <v>-88</v>
+      </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="n">
-        <v>-88</v>
-      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2045,82 +1868,73 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1749</v>
+        <v>9862</v>
       </c>
       <c r="C26" t="n">
-        <v>8113</v>
+        <v>2134</v>
       </c>
       <c r="D26" t="n">
-        <v>9862</v>
+        <v>-861</v>
       </c>
       <c r="E26" t="n">
-        <v>2134</v>
+        <v>1710</v>
       </c>
       <c r="F26" t="n">
-        <v>-861</v>
+        <v>4960</v>
       </c>
       <c r="G26" t="n">
-        <v>1710</v>
+        <v>6670</v>
       </c>
       <c r="H26" t="n">
-        <v>4960</v>
+        <v>3842</v>
       </c>
       <c r="I26" t="n">
-        <v>6670</v>
+        <v>3610</v>
       </c>
       <c r="J26" t="n">
-        <v>3842</v>
+        <v>3288</v>
       </c>
       <c r="K26" t="n">
-        <v>3610</v>
+        <v>11593</v>
       </c>
       <c r="L26" t="n">
-        <v>3288</v>
+        <v>14881</v>
       </c>
       <c r="M26" t="n">
-        <v>11593</v>
+        <v>3990</v>
       </c>
       <c r="N26" t="n">
-        <v>14881</v>
+        <v>6476</v>
       </c>
       <c r="O26" t="n">
-        <v>3990</v>
+        <v>5135</v>
       </c>
       <c r="P26" t="n">
-        <v>6476</v>
+        <v>8375</v>
       </c>
       <c r="Q26" t="n">
-        <v>5135</v>
+        <v>13510</v>
       </c>
       <c r="R26" t="n">
-        <v>8375</v>
+        <v>2730</v>
       </c>
       <c r="S26" t="n">
-        <v>13510</v>
+        <v>4276</v>
       </c>
       <c r="T26" t="n">
-        <v>2730</v>
+        <v>3105</v>
       </c>
       <c r="U26" t="n">
-        <v>4276</v>
+        <v>10568</v>
       </c>
       <c r="V26" t="n">
-        <v>3105</v>
-      </c>
-      <c r="W26" t="n">
-        <v>10568</v>
-      </c>
-      <c r="X26" t="n">
         <v>13673</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>2054</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>basic net income per common share:</t>
+          <t>net income per common share:</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -2144,14 +1958,11 @@
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>net income per common share:</t>
+          <t>basic net income per common share:</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -2175,9 +1986,6 @@
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2186,76 +1994,67 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.59</v>
+        <v>3.29</v>
       </c>
       <c r="C29" t="n">
-        <v>2.7</v>
+        <v>0.72</v>
       </c>
       <c r="D29" t="n">
-        <v>3.29</v>
+        <v>-0.29</v>
       </c>
       <c r="E29" t="n">
-        <v>0.72</v>
+        <v>0.58</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.29</v>
+        <v>1.7</v>
       </c>
       <c r="G29" t="n">
-        <v>0.58</v>
+        <v>2.28</v>
       </c>
       <c r="H29" t="n">
-        <v>1.7</v>
+        <v>1.34</v>
       </c>
       <c r="I29" t="n">
-        <v>2.28</v>
+        <v>1.27</v>
       </c>
       <c r="J29" t="n">
-        <v>1.34</v>
+        <v>1.16</v>
       </c>
       <c r="K29" t="n">
-        <v>1.27</v>
+        <v>4.06</v>
       </c>
       <c r="L29" t="n">
-        <v>1.16</v>
+        <v>5.22</v>
       </c>
       <c r="M29" t="n">
-        <v>4.06</v>
+        <v>1.41</v>
       </c>
       <c r="N29" t="n">
-        <v>5.22</v>
+        <v>2.29</v>
       </c>
       <c r="O29" t="n">
-        <v>1.41</v>
+        <v>1.81</v>
       </c>
       <c r="P29" t="n">
-        <v>2.29</v>
+        <v>2.96</v>
       </c>
       <c r="Q29" t="n">
-        <v>1.81</v>
+        <v>4.77</v>
       </c>
       <c r="R29" t="n">
-        <v>2.96</v>
+        <v>0.97</v>
       </c>
       <c r="S29" t="n">
-        <v>4.77</v>
+        <v>1.53</v>
       </c>
       <c r="T29" t="n">
-        <v>0.97</v>
+        <v>1.11</v>
       </c>
       <c r="U29" t="n">
-        <v>1.53</v>
+        <v>3.79</v>
       </c>
       <c r="V29" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="W29" t="n">
-        <v>3.79</v>
-      </c>
-      <c r="X29" t="n">
         <v>4.9</v>
-      </c>
-      <c r="Y29" t="n">
-        <v>0.75</v>
       </c>
     </row>
     <row r="30">
@@ -2285,9 +2084,6 @@
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2296,76 +2092,67 @@
         </is>
       </c>
       <c r="B31" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-0.29</v>
+      </c>
+      <c r="E31" t="n">
         <v>0.58</v>
       </c>
-      <c r="C31" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="D31" t="n">
-        <v>3.28</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.72</v>
-      </c>
       <c r="F31" t="n">
-        <v>-0.29</v>
+        <v>1.68</v>
       </c>
       <c r="G31" t="n">
-        <v>0.58</v>
+        <v>2.26</v>
       </c>
       <c r="H31" t="n">
-        <v>1.68</v>
+        <v>1.33</v>
       </c>
       <c r="I31" t="n">
-        <v>2.26</v>
+        <v>1.26</v>
       </c>
       <c r="J31" t="n">
-        <v>1.33</v>
+        <v>1.15</v>
       </c>
       <c r="K31" t="n">
-        <v>1.26</v>
+        <v>4.040000000000001</v>
       </c>
       <c r="L31" t="n">
-        <v>1.15</v>
+        <v>5.19</v>
       </c>
       <c r="M31" t="n">
-        <v>4.040000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="N31" t="n">
-        <v>5.19</v>
+        <v>2.27</v>
       </c>
       <c r="O31" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="P31" t="n">
-        <v>2.27</v>
+        <v>2.95</v>
       </c>
       <c r="Q31" t="n">
-        <v>1.8</v>
+        <v>4.75</v>
       </c>
       <c r="R31" t="n">
-        <v>2.95</v>
+        <v>0.97</v>
       </c>
       <c r="S31" t="n">
-        <v>4.75</v>
+        <v>1.52</v>
       </c>
       <c r="T31" t="n">
-        <v>0.97</v>
+        <v>1.11</v>
       </c>
       <c r="U31" t="n">
-        <v>1.52</v>
+        <v>3.76</v>
       </c>
       <c r="V31" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="W31" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="X31" t="n">
         <v>4.87</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>0.74</v>
       </c>
     </row>
     <row r="32">
@@ -2395,9 +2182,6 @@
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr"/>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2406,76 +2190,67 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2981</v>
+        <v>2995</v>
       </c>
       <c r="C33" t="n">
-        <v>14</v>
+        <v>2950</v>
       </c>
       <c r="D33" t="n">
-        <v>2995</v>
+        <v>2946</v>
       </c>
       <c r="E33" t="n">
-        <v>2950</v>
+        <v>2924</v>
       </c>
       <c r="F33" t="n">
-        <v>2946</v>
+        <v>5</v>
       </c>
       <c r="G33" t="n">
-        <v>2924</v>
+        <v>2929</v>
       </c>
       <c r="H33" t="n">
-        <v>5</v>
+        <v>2869</v>
       </c>
       <c r="I33" t="n">
-        <v>2929</v>
+        <v>2853</v>
       </c>
       <c r="J33" t="n">
-        <v>2869</v>
+        <v>2843</v>
       </c>
       <c r="K33" t="n">
-        <v>2853</v>
+        <v>7</v>
       </c>
       <c r="L33" t="n">
-        <v>2843</v>
+        <v>2850</v>
       </c>
       <c r="M33" t="n">
+        <v>2831</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2832</v>
+      </c>
+      <c r="O33" t="n">
+        <v>2833</v>
+      </c>
+      <c r="P33" t="n">
+        <v>-2</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>2831</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2815</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2799</v>
+      </c>
+      <c r="T33" t="n">
+        <v>2785</v>
+      </c>
+      <c r="U33" t="n">
         <v>7</v>
       </c>
-      <c r="N33" t="n">
-        <v>2850</v>
-      </c>
-      <c r="O33" t="n">
-        <v>2831</v>
-      </c>
-      <c r="P33" t="n">
-        <v>2832</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>2833</v>
-      </c>
-      <c r="R33" t="n">
-        <v>-2</v>
-      </c>
-      <c r="S33" t="n">
-        <v>2831</v>
-      </c>
-      <c r="T33" t="n">
-        <v>2815</v>
-      </c>
-      <c r="U33" t="n">
-        <v>2799</v>
-      </c>
       <c r="V33" t="n">
-        <v>2785</v>
-      </c>
-      <c r="W33" t="n">
-        <v>7</v>
-      </c>
-      <c r="X33" t="n">
         <v>2792</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>2754</v>
       </c>
     </row>
     <row r="34">
@@ -2485,76 +2260,67 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2996</v>
+        <v>3010</v>
       </c>
       <c r="C34" t="n">
-        <v>14</v>
+        <v>2967</v>
       </c>
       <c r="D34" t="n">
-        <v>3010</v>
+        <v>2946</v>
       </c>
       <c r="E34" t="n">
-        <v>2967</v>
+        <v>2941</v>
       </c>
       <c r="F34" t="n">
-        <v>2946</v>
+        <v>4</v>
       </c>
       <c r="G34" t="n">
-        <v>2941</v>
+        <v>2945</v>
       </c>
       <c r="H34" t="n">
-        <v>4</v>
+        <v>2886</v>
       </c>
       <c r="I34" t="n">
-        <v>2945</v>
+        <v>2869</v>
       </c>
       <c r="J34" t="n">
-        <v>2886</v>
+        <v>2861</v>
       </c>
       <c r="K34" t="n">
-        <v>2869</v>
+        <v>7</v>
       </c>
       <c r="L34" t="n">
-        <v>2861</v>
+        <v>2868</v>
       </c>
       <c r="M34" t="n">
-        <v>7</v>
+        <v>2849</v>
       </c>
       <c r="N34" t="n">
-        <v>2868</v>
+        <v>2848</v>
       </c>
       <c r="O34" t="n">
         <v>2849</v>
       </c>
       <c r="P34" t="n">
-        <v>2848</v>
+        <v>-2</v>
       </c>
       <c r="Q34" t="n">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="R34" t="n">
-        <v>-2</v>
+        <v>2829</v>
       </c>
       <c r="S34" t="n">
-        <v>2847</v>
+        <v>2812</v>
       </c>
       <c r="T34" t="n">
-        <v>2829</v>
+        <v>2797</v>
       </c>
       <c r="U34" t="n">
-        <v>2812</v>
+        <v>8</v>
       </c>
       <c r="V34" t="n">
-        <v>2797</v>
-      </c>
-      <c r="W34" t="n">
-        <v>8</v>
-      </c>
-      <c r="X34" t="n">
         <v>2805</v>
-      </c>
-      <c r="Y34" t="n">
-        <v>2765</v>
       </c>
     </row>
     <row r="35">
@@ -2564,76 +2330,67 @@
         </is>
       </c>
       <c r="B35" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="D35" t="n">
         <v>0</v>
       </c>
-      <c r="C35" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="D35" t="n">
-        <v>2.04</v>
-      </c>
       <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
         <v>2.08</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="I35" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="n">
+      <c r="J35" t="n">
         <v>0</v>
       </c>
-      <c r="H35" t="n">
-        <v>2.08</v>
-      </c>
-      <c r="I35" t="n">
-        <v>2.08</v>
-      </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>2.12</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="M35" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="N35" t="n">
         <v>0</v>
       </c>
-      <c r="L35" t="n">
+      <c r="O35" t="n">
         <v>0</v>
       </c>
-      <c r="M35" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="N35" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="O35" t="n">
+      <c r="P35" t="n">
         <v>2.16</v>
       </c>
-      <c r="P35" t="n">
+      <c r="Q35" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="R35" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="S35" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="T35" t="n">
         <v>0</v>
       </c>
-      <c r="R35" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="S35" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="T35" t="n">
+      <c r="U35" t="n">
         <v>2.2</v>
       </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
       <c r="V35" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" t="n">
         <v>2.2</v>
-      </c>
-      <c r="X35" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="Y35" t="n">
-        <v>2.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>